<commit_message>
add 'git branch -r'
</commit_message>
<xml_diff>
--- a/Git-Command.xlsx
+++ b/Git-Command.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="175">
   <si>
     <t>选项</t>
   </si>
@@ -1515,6 +1515,14 @@
   </si>
   <si>
     <t>git rebase master server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git branch -r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看所有的远程分支</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1750,7 +1758,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1769,6 +1777,30 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1778,29 +1810,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2096,10 +2107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2111,18 +2122,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
@@ -2269,18 +2280,18 @@
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
@@ -2375,11 +2386,11 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="11"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="4" t="s">
@@ -2467,18 +2478,18 @@
       <c r="C40" s="5"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="16"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="11"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
@@ -2565,18 +2576,18 @@
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="8"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="16"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="11"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="5" t="s">
@@ -2628,18 +2639,18 @@
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="8"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="16"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B62" s="10"/>
-      <c r="C62" s="11"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="8"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="5" t="s">
@@ -2659,7 +2670,7 @@
       </c>
       <c r="C64" s="5"/>
     </row>
-    <row r="65" spans="1:4" ht="48">
+    <row r="65" spans="1:3" ht="48">
       <c r="A65" s="5" t="s">
         <v>113</v>
       </c>
@@ -2670,7 +2681,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:3">
       <c r="A66" s="5" t="s">
         <v>116</v>
       </c>
@@ -2681,7 +2692,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="48">
+    <row r="67" spans="1:3" ht="48">
       <c r="A67" s="5" t="s">
         <v>118</v>
       </c>
@@ -2692,7 +2703,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:3">
       <c r="A68" s="5" t="s">
         <v>121</v>
       </c>
@@ -2701,14 +2712,14 @@
       </c>
       <c r="C68" s="5"/>
     </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="12" t="s">
+    <row r="69" spans="1:3">
+      <c r="A69" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B69" s="10"/>
-      <c r="C69" s="11"/>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="B69" s="7"/>
+      <c r="C69" s="8"/>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="5" t="s">
         <v>126</v>
       </c>
@@ -2717,7 +2728,7 @@
       </c>
       <c r="C70" s="5"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:3">
       <c r="A71" s="5" t="s">
         <v>136</v>
       </c>
@@ -2726,7 +2737,7 @@
       </c>
       <c r="C71" s="5"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:3">
       <c r="A72" s="5" t="s">
         <v>128</v>
       </c>
@@ -2735,7 +2746,7 @@
       </c>
       <c r="C72" s="5"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:3">
       <c r="A73" s="5" t="s">
         <v>130</v>
       </c>
@@ -2744,207 +2755,216 @@
       </c>
       <c r="C73" s="5"/>
     </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="12" t="s">
+    <row r="74" spans="1:3">
+      <c r="A74" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B74" s="10"/>
-      <c r="C74" s="11"/>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="B74" s="7"/>
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C75" s="5"/>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C75" s="5"/>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="12" t="s">
+      <c r="C76" s="5"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="11"/>
-    </row>
-    <row r="77" spans="1:4" ht="23.25">
-      <c r="A77" s="5" t="s">
+      <c r="B77" s="7"/>
+      <c r="C77" s="8"/>
+    </row>
+    <row r="78" spans="1:3" ht="23.25">
+      <c r="A78" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C77" s="5"/>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="5" t="s">
+      <c r="C78" s="5"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C78" s="5"/>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="12" t="s">
+      <c r="C79" s="5"/>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B79" s="10"/>
-      <c r="C79" s="11"/>
-    </row>
-    <row r="80" spans="1:4" ht="72">
-      <c r="A80" s="5" t="s">
+      <c r="B80" s="7"/>
+      <c r="C80" s="8"/>
+    </row>
+    <row r="81" spans="1:4" ht="72">
+      <c r="A81" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C81" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D80" s="5"/>
-    </row>
-    <row r="81" spans="1:4" ht="26.25" customHeight="1">
-      <c r="A81" s="13" t="s">
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="1:4" ht="26.25" customHeight="1">
+      <c r="A82" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="B81" s="10"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="5"/>
-    </row>
-    <row r="82" spans="1:4" ht="24">
-      <c r="A82" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C82" s="5"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="8"/>
       <c r="D82" s="5"/>
     </row>
     <row r="83" spans="1:4" ht="24">
       <c r="A83" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="1:4" ht="24">
+      <c r="A84" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C84" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D83" s="5"/>
-    </row>
-    <row r="84" spans="1:4" ht="47.25">
-      <c r="A84" s="5" t="s">
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="1:4" ht="47.25">
+      <c r="A85" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C85" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="24">
-      <c r="A85" s="5" t="s">
+    <row r="86" spans="1:4" ht="24">
+      <c r="A86" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C85" s="5"/>
-    </row>
-    <row r="86" spans="1:4" ht="228">
-      <c r="A86" s="5" t="s">
+      <c r="C86" s="5"/>
+    </row>
+    <row r="87" spans="1:4" ht="228">
+      <c r="A87" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="12" t="s">
+    <row r="88" spans="1:4">
+      <c r="A88" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B87" s="10"/>
-      <c r="C87" s="11"/>
-    </row>
-    <row r="88" spans="1:4" ht="36">
-      <c r="A88" s="5" t="s">
+      <c r="B88" s="7"/>
+      <c r="C88" s="8"/>
+    </row>
+    <row r="89" spans="1:4" ht="36">
+      <c r="A89" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C89" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="12" t="s">
+    <row r="90" spans="1:4">
+      <c r="A90" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B89" s="10"/>
-      <c r="C89" s="11"/>
-    </row>
-    <row r="90" spans="1:4" ht="39.75" customHeight="1">
-      <c r="A90" s="14" t="s">
+      <c r="B90" s="7"/>
+      <c r="C90" s="8"/>
+    </row>
+    <row r="91" spans="1:4" ht="39.75" customHeight="1">
+      <c r="A91" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B90" s="15"/>
-      <c r="C90" s="16"/>
-    </row>
-    <row r="91" spans="1:4" ht="96">
-      <c r="A91" s="5"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="36">
-      <c r="A92" s="5" t="s">
-        <v>168</v>
-      </c>
+      <c r="B91" s="10"/>
+      <c r="C91" s="11"/>
+    </row>
+    <row r="92" spans="1:4" ht="96">
+      <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="36">
+      <c r="A93" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="5" t="s">
+    <row r="94" spans="1:4">
+      <c r="A94" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C94" s="5" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A90:C90"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A62:C62"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A90:C90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A77:C77"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add git reset command
</commit_message>
<xml_diff>
--- a/Git-Command.xlsx
+++ b/Git-Command.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="203">
   <si>
     <t>选项</t>
   </si>
@@ -1742,6 +1742,16 @@
 the url needs to be something like ssh://git@github.com/YourDirectory/YourProject.git; if you don't see git@github.com, use
 git remote set-url origin git://github.com/YourDirectory/YourProject.git
 to set it right. Or you could use the github app to check and set the Primary Remote Repository url in the settings panel of your particular repository.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git reset --hard &lt;commit_id&gt;
+git push origin HEAD --force</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 回滚到某一版本(SHA-1)
+2. 把回滚的版本更新到服务器端(强制设置服务器端HEAD为回滚的SHA-1)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1999,6 +2009,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2011,15 +2033,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2027,9 +2040,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2336,10 +2346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2351,18 +2361,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
@@ -2509,18 +2519,18 @@
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
@@ -2615,11 +2625,11 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
@@ -2707,18 +2717,18 @@
       <c r="C40" s="5"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="9"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="9"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="5" t="s">
@@ -2805,18 +2815,18 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="9"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="13"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="5" t="s">
@@ -2868,18 +2878,18 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="9"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="13"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="12"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="9"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="5" t="s">
@@ -2942,11 +2952,11 @@
       <c r="C68" s="5"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B69" s="11"/>
-      <c r="C69" s="12"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="9"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="5" t="s">
@@ -2985,11 +2995,11 @@
       <c r="C73" s="5"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A74" s="13" t="s">
+      <c r="A74" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B74" s="11"/>
-      <c r="C74" s="12"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="9"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="5" t="s">
@@ -3010,11 +3020,11 @@
       <c r="C76" s="5"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A77" s="13" t="s">
+      <c r="A77" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B77" s="11"/>
-      <c r="C77" s="12"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3" ht="23.25" x14ac:dyDescent="0.15">
       <c r="A78" s="5" t="s">
@@ -3035,11 +3045,11 @@
       <c r="C79" s="5"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A80" s="13" t="s">
+      <c r="A80" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B80" s="11"/>
-      <c r="C80" s="12"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="9"/>
     </row>
     <row r="81" spans="1:4" ht="72" x14ac:dyDescent="0.15">
       <c r="A81" s="5" t="s">
@@ -3054,11 +3064,11 @@
       <c r="D81" s="5"/>
     </row>
     <row r="82" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="B82" s="11"/>
-      <c r="C82" s="12"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
       <c r="D82" s="5"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
@@ -3115,11 +3125,11 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="12"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="9"/>
     </row>
     <row r="89" spans="1:4" ht="36" x14ac:dyDescent="0.15">
       <c r="A89" s="5" t="s">
@@ -3133,18 +3143,18 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B90" s="11"/>
-      <c r="C90" s="12"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="9"/>
     </row>
     <row r="91" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="14" t="s">
+      <c r="A91" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="B91" s="15"/>
-      <c r="C91" s="16"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="17"/>
     </row>
     <row r="92" spans="1:4" ht="96" x14ac:dyDescent="0.15">
       <c r="A92" s="5"/>
@@ -3174,11 +3184,11 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="B96" s="8"/>
-      <c r="C96" s="9"/>
+      <c r="B96" s="12"/>
+      <c r="C96" s="13"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A97" s="5" t="s">
@@ -3243,11 +3253,11 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A104" s="7" t="s">
+      <c r="A104" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B104" s="8"/>
-      <c r="C104" s="9"/>
+      <c r="B104" s="12"/>
+      <c r="C104" s="13"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A105" s="5"/>
@@ -3289,13 +3299,16 @@
         <v>200</v>
       </c>
     </row>
+    <row r="111" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A111" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A82:C82"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A77:C77"/>
     <mergeCell ref="A104:C104"/>
     <mergeCell ref="A96:C96"/>
     <mergeCell ref="A1:C1"/>
@@ -3312,6 +3325,11 @@
     <mergeCell ref="A90:C90"/>
     <mergeCell ref="A91:C91"/>
     <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A77:C77"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>